<commit_message>
Enable support for Hindi and other languages in imported questions
Updates question import functionality to support Hindi and other languages in .xlsx, .csv, and .docx formats in `import-questions.tsx`, `sample-questions.csv`, `sample-questions.txt`, and `sample-questions.xlsx`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 788c0ad7-8efe-4745-8b9e-03ef3d8882d6
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/35d73528-0c3c-4528-90b6-58a81f7f28df/eb183857-0c22-4003-a2ef-fb60d2216c37.jpg
</commit_message>
<xml_diff>
--- a/public/templates/sample-questions.xlsx
+++ b/public/templates/sample-questions.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -528,9 +528,52 @@
         <v>Gravity is a force that attracts objects with mass towards each other, with the strength proportional to their masses and inversely proportional to the square of the distance between them.</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>mcq</v>
+      </c>
+      <c r="B7" t="str">
+        <v>भारत की राजधानी क्या है?</v>
+      </c>
+      <c r="C7" t="str">
+        <v>A:मुंबई,B:दिल्ली,C:कोलकाता,D:चेन्नई</v>
+      </c>
+      <c r="D7" t="str">
+        <v>b</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="str">
+        <v>दिल्ली भारत की राजधानी है</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>fillblank</v>
+      </c>
+      <c r="B8" t="str">
+        <v>गणित में π का मान लगभग ___ होता है।</v>
+      </c>
+      <c r="D8" t="str">
+        <v>3.14159</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="str">
+        <v>3.14159 गणित में π का लगभग मान है</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>